<commit_message>
Iniciando o SQL e MLR
</commit_message>
<xml_diff>
--- a/PROJETO.xlsx
+++ b/PROJETO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="105">
   <si>
     <t>Cronograma do Projeto de FBD</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Progresso Geral</t>
   </si>
   <si>
-    <t>13.5%</t>
-  </si>
-  <si>
     <t>Período</t>
   </si>
   <si>
@@ -293,10 +290,52 @@
     <t>Dúvida</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>4 dias</t>
+  </si>
+  <si>
+    <t>Business Edereco</t>
+  </si>
+  <si>
+    <t>Business Limpesa</t>
+  </si>
+  <si>
+    <t>Business Revisao</t>
+  </si>
+  <si>
+    <t>Business Veículo</t>
+  </si>
+  <si>
+    <t>Business Cliente + PF e PJ</t>
+  </si>
+  <si>
+    <t>Business Categorias + Automovel + Camionetas de Carga + Camionetas de Passageiros</t>
+  </si>
+  <si>
+    <t>Business Motoristas</t>
+  </si>
+  <si>
+    <t>Business Sede/Filial</t>
+  </si>
+  <si>
+    <t>Business Usuário</t>
+  </si>
+  <si>
+    <t>Business Reserva</t>
+  </si>
+  <si>
+    <t>Business Controle Financeiro</t>
+  </si>
+  <si>
+    <t>Business Formas de Pagamentos</t>
+  </si>
+  <si>
+    <t>Business Locação</t>
+  </si>
+  <si>
+    <t>Fachada</t>
+  </si>
+  <si>
+    <t>26.3%</t>
   </si>
 </sst>
 </file>
@@ -800,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK55"/>
+  <dimension ref="A1:AMK68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -864,41 +903,41 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="G10" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D11" s="8">
         <v>43390</v>
@@ -907,18 +946,18 @@
         <v>43393</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D12" s="8">
         <v>43394</v>
@@ -927,18 +966,18 @@
         <v>43402</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="8">
         <v>43400</v>
@@ -947,38 +986,37 @@
         <v>43401</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="8">
-        <v>43408</v>
-      </c>
-      <c r="E14" s="8">
-        <v>43408</v>
-      </c>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="8">
         <v>43407</v>
@@ -987,35 +1025,35 @@
         <v>43408</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="9">
         <v>43421</v>
@@ -1024,18 +1062,18 @@
         <v>43422</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D18" s="9">
         <v>43423</v>
@@ -1044,18 +1082,18 @@
         <v>43423</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="9">
         <v>43423</v>
@@ -1064,18 +1102,18 @@
         <v>43423</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="9">
         <v>43423</v>
@@ -1084,18 +1122,18 @@
         <v>43423</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="9">
         <v>43423</v>
@@ -1104,18 +1142,18 @@
         <v>43423</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D22" s="9">
         <v>43423</v>
@@ -1124,21 +1162,21 @@
         <v>43423</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="9">
         <v>43424</v>
@@ -1147,21 +1185,21 @@
         <v>43424</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24" s="9">
         <v>43424</v>
@@ -1170,18 +1208,18 @@
         <v>43424</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D25" s="9">
         <v>43424</v>
@@ -1190,18 +1228,18 @@
         <v>43424</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D26" s="9">
         <v>43424</v>
@@ -1210,18 +1248,18 @@
         <v>43424</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D27" s="9">
         <v>43424</v>
@@ -1230,18 +1268,18 @@
         <v>43424</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="9">
         <v>43424</v>
@@ -1250,18 +1288,18 @@
         <v>43424</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D29" s="9">
         <v>43424</v>
@@ -1270,18 +1308,18 @@
         <v>43424</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D30" s="9">
         <v>43424</v>
@@ -1290,359 +1328,541 @@
         <v>43424</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="9"/>
       <c r="F31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>44</v>
+        <v>97</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>99</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>26</v>
+        <v>66</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>52</v>
+        <v>102</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>53</v>
+        <v>103</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>33</v>
+      <c r="F68" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>